<commit_message>
Update list with company name and url seperately
</commit_message>
<xml_diff>
--- a/list.xlsx
+++ b/list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Poojitha Sri\Job_Docs\Git\NotifyCareerPortalsUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6608685-35C2-4E9C-9480-074EAAE77E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C97E516-43B6-4D56-8529-A7A98318E0A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,73 +20,127 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>company</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>update</t>
   </si>
   <si>
-    <t>https://www.tu-chemnitz.de/career-service/jobboerse/index.php</t>
-  </si>
-  <si>
     <t>Could not reach host. Are you offline?</t>
   </si>
   <si>
-    <t>https://jobs.bosch.de/</t>
-  </si>
-  <si>
-    <t>https://jobs.siemens.com/careers?location=germany&amp;pid=563156124122350&amp;domain=siemens.com&amp;sort_by=relevance&amp;triggerGoButton=false</t>
-  </si>
-  <si>
-    <t>https://www.tesla.com/careers/search/?site=DE&amp;type=1</t>
-  </si>
-  <si>
-    <t>https://careers.audi.com/desktop.html#/SEARCH/SIMPLE/</t>
-  </si>
-  <si>
-    <t>https://career.iav.com/en/</t>
-  </si>
-  <si>
-    <t>https://www.intenta-automotive.de/en/career.html</t>
-  </si>
-  <si>
-    <t>https://www.fdtech.de/career-and-jobs/#46fab92f5345</t>
-  </si>
-  <si>
-    <t>https://jobs.mercedes-benz.com/enUS</t>
-  </si>
-  <si>
-    <t>https://jobs.porsche.com/index.php?ac=search_result&amp;search_criterion_entry_level%5B%5D=5&amp;search_criterion_channel%5B%5D=12</t>
-  </si>
-  <si>
-    <t>https://jobs.fraunhofer.de/go/All-Job-Offers/5366301/</t>
-  </si>
-  <si>
-    <t>https://unicontrol.de/en/applicants</t>
-  </si>
-  <si>
-    <t>https://jobs.volkswagen-group.com/Volkswagen-Group-Services/search/?locale=de_DE</t>
-  </si>
-  <si>
-    <t>https://www.akkodis.com/en-us/careers/job-results</t>
-  </si>
-  <si>
-    <t>https://karriere.hoermann-gruppe.com/en/</t>
-  </si>
-  <si>
-    <t>https://www.edag.com/en/career/vacancies</t>
-  </si>
-  <si>
-    <t>https://www.bmwgroup.jobs/de/en.html</t>
+    <t>Company_name</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>BOSCH</t>
+  </si>
+  <si>
+    <t>IAV</t>
+  </si>
+  <si>
+    <t>FDTECH</t>
+  </si>
+  <si>
+    <t>SIEMENS</t>
+  </si>
+  <si>
+    <t>PORSCHE</t>
+  </si>
+  <si>
+    <t>TESLA</t>
+  </si>
+  <si>
+    <t>AUDI</t>
+  </si>
+  <si>
+    <t>FRAUNHOFER</t>
+  </si>
+  <si>
+    <t>AKKODIS</t>
+  </si>
+  <si>
+    <t>EDAG</t>
+  </si>
+  <si>
+    <t>INTENTA</t>
+  </si>
+  <si>
+    <t>MERCEDES</t>
+  </si>
+  <si>
+    <t>VOLKSWAGEN</t>
+  </si>
+  <si>
+    <t>HOERMANN</t>
+  </si>
+  <si>
+    <t>TUC</t>
+  </si>
+  <si>
+    <t>BMW</t>
+  </si>
+  <si>
+    <t>UNICONTROL</t>
+  </si>
+  <si>
+    <t>https://jobs.siemens.com/careers?location=any&amp;pid=563156124196614&amp;domain=siemens.com&amp;sort_by=relevance&amp;triggerGoButton=false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://jobs.bosch.de/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.tu-chemnitz.de/career-service/jobboerse/index.php </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.tesla.com/careers/search/?site=DE&amp;type=1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://careers.audi.com/desktop.html#/SEARCH/SIMPLE/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://career.iav.com/en/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.intenta-automotive.de/en/career.html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.fdtech.de/career-and-jobs/#46fab92f5345 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://jobs.mercedes-benz.com/enUS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://jobs.porsche.com/index.php?ac=search_result&amp;search_criterion_entry_level%5B%5D=5&amp;search_criterion_channel%5B%5D=12 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://jobs.fraunhofer.de/go/All-Job-Offers/5366301/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://unicontrol.de/en/applicants </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://jobs.volkswagen-group.com/Volkswagen-Group-Services/search/?locale=de_DE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.akkodis.com/en-us/careers/job-results </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://karriere.hoermann-gruppe.com/en/ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.edag.com/en/career/vacancies </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.bmwgroup.jobs/de/en.html </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +152,22 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -132,16 +202,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -442,115 +516,189 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="124.6328125" customWidth="1"/>
-    <col min="2" max="2" width="50.453125" customWidth="1"/>
+    <col min="1" max="1" width="22.08984375" customWidth="1"/>
+    <col min="2" max="2" width="124.6328125" customWidth="1"/>
+    <col min="3" max="3" width="50.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B3" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B7" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="B9" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="B11" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="B12" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B15" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B16" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>19</v>
       </c>
+      <c r="B18" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{8AB7CA27-42C7-4897-AB72-E947BFA94677}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{CAF575D5-3F20-4465-970F-D8A433B0C303}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{72663E4D-D9A9-41C1-B572-D0BF8ACE9FAE}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{A9822F02-0FB1-4566-B1B3-218C0DE22154}"/>
+    <hyperlink ref="B6" r:id="rId5" location="/SEARCH/SIMPLE/ " xr:uid="{5EA94F5B-A2A9-43D2-9E7E-E2F3CF2AEDC0}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{46AF2A31-F69A-4D47-9A45-6B2F1CBB196A}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{B5864CA3-FF91-436A-BAD1-2C90139A9B12}"/>
+    <hyperlink ref="B9" r:id="rId8" location="46fab92f5345 " xr:uid="{5C730DD3-12DD-4C4B-AF74-408625CDA08A}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{310DCF31-DF2F-4268-A6B0-AFE8419D6C34}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{FF46DAC7-7C44-4443-B926-A3E2B8DBB963}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{D4C3EA94-D5CD-4A18-8853-5566AF76F0E4}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{740A2FB5-F609-458F-8553-5DF35229E353}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{6994FA4D-0703-4DEB-A574-A56D01C8C2D3}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{07B0E0AC-F2EB-4874-887F-669E34FC1E81}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{969193DC-1E98-4465-8CF6-A69A8A8423D3}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{D1EE638A-1ABB-4E57-B02F-F3CE35D57B6C}"/>
+    <hyperlink ref="B18" r:id="rId17" xr:uid="{55860669-A8A1-40A5-A78F-6C62F3518D35}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>